<commit_message>
add other fields generators
</commit_message>
<xml_diff>
--- a/src/test/resources/CreatedUserInformation.xlsx
+++ b/src/test/resources/CreatedUserInformation.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20368"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B3518F-5EE4-47C5-8D50-1388EAFE148F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB9011B-5262-4BEB-A096-CCCF3EC14993}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Deactive" sheetId="1" r:id="rId1"/>
-    <sheet name="Active" sheetId="2" r:id="rId2"/>
+    <sheet name="registered" sheetId="1" r:id="rId1"/>
+    <sheet name="jhi_user" sheetId="2" r:id="rId2"/>
+    <sheet name="customer" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>ssnNumber</t>
   </si>
@@ -47,77 +48,46 @@
     <t>newPassword</t>
   </si>
   <si>
-    <t>111-111-1111</t>
-  </si>
-  <si>
-    <t>194-20-1563</t>
-  </si>
-  <si>
-    <t>Sherley</t>
-  </si>
-  <si>
-    <t>Weber</t>
-  </si>
-  <si>
-    <t>Apt. 948 4156 Gerlach Shoal, West Roseannahaven, WY 78532</t>
-  </si>
-  <si>
-    <t>betsey.gorczany</t>
-  </si>
-  <si>
-    <t>jenine.oconner@yahoo.com</t>
-  </si>
-  <si>
-    <t>zQ3*Blq</t>
-  </si>
-  <si>
-    <t>717-92-9443</t>
-  </si>
-  <si>
-    <t>Franklyn</t>
-  </si>
-  <si>
-    <t>Pfeffer</t>
-  </si>
-  <si>
-    <t>Suite 151 18823 Benedict Expressway, Port Renato, AR 77128</t>
-  </si>
-  <si>
-    <t>sammie.kirlin</t>
-  </si>
-  <si>
-    <t>donnell.marvin@yahoo.com</t>
-  </si>
-  <si>
-    <t>sI6~JN1</t>
-  </si>
-  <si>
-    <t>589-38-2580</t>
-  </si>
-  <si>
-    <t>Gaylord</t>
-  </si>
-  <si>
-    <t>Turcotte</t>
-  </si>
-  <si>
-    <t>Apt. 811 913 Edmund Forge, Lake Dennis, MT 80670</t>
-  </si>
-  <si>
-    <t>malik.stark</t>
-  </si>
-  <si>
-    <t>chuck.bayer@yahoo.com</t>
-  </si>
-  <si>
-    <t>vB3==fH</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>activation</t>
+  </si>
+  <si>
+    <t>profiles</t>
+  </si>
+  <si>
+    <t>zipcode</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>account1</t>
+  </si>
+  <si>
+    <t>account2</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>zelleEnrolled</t>
+  </si>
+  <si>
+    <t>createdDate</t>
+  </si>
+  <si>
+    <t>zipCode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,25 +406,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.77734375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="52.44140625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.21875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="24.5546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,94 +442,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -565,12 +473,167 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A8C0A6-A5D7-4843-BF59-F8CA009F27C6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:N1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BFD007-6D85-4BB6-B9BF-B15426A563F8}">
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
work on excel utilities
</commit_message>
<xml_diff>
--- a/src/test/resources/CreatedUserInformation.xlsx
+++ b/src/test/resources/CreatedUserInformation.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB9011B-5262-4BEB-A096-CCCF3EC14993}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD6CF18-D2B0-477C-BB2F-DDBBDEB7CA66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registered" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>ssnNumber</t>
   </si>
@@ -45,9 +45,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>newPassword</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -82,12 +79,82 @@
   </si>
   <si>
     <t>zipCode</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Schneider</t>
+  </si>
+  <si>
+    <t>511-434-3547</t>
+  </si>
+  <si>
+    <t>18752</t>
+  </si>
+  <si>
+    <t>19609 Morgan Drive</t>
+  </si>
+  <si>
+    <t>South Ninfaside</t>
+  </si>
+  <si>
+    <t>375-15-7057</t>
+  </si>
+  <si>
+    <t>amanda.rodriguez</t>
+  </si>
+  <si>
+    <t>Wallace</t>
+  </si>
+  <si>
+    <t>cC5;–9Z</t>
+  </si>
+  <si>
+    <t>432-131-5405</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>sal.fisher@hotmail.com</t>
+  </si>
+  <si>
+    <t>Mercy</t>
+  </si>
+  <si>
+    <t>Mante</t>
+  </si>
+  <si>
+    <t>30495</t>
+  </si>
+  <si>
+    <t>28037 Gulgowski Shore</t>
+  </si>
+  <si>
+    <t>588-697-5116</t>
+  </si>
+  <si>
+    <t>Darrickshire</t>
+  </si>
+  <si>
+    <t>364-66-8818</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>claudette.jerde</t>
+  </si>
+  <si>
+    <t>sherley.moen@yahoo.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -406,26 +473,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.6640625" customWidth="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="3.88671875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -442,19 +509,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -463,7 +530,45 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -476,24 +581,24 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:N1048576"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.21875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="5.77734375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -510,19 +615,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>5</v>
@@ -531,13 +636,13 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -549,29 +654,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BFD007-6D85-4BB6-B9BF-B15426A563F8}">
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.21875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="5.77734375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="2.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="17" max="18" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -588,16 +693,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -609,28 +714,28 @@
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add methods to take last user who has been registered correct configuration file
</commit_message>
<xml_diff>
--- a/src/test/resources/CreatedUserInformation.xlsx
+++ b/src/test/resources/CreatedUserInformation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD6CF18-D2B0-477C-BB2F-DDBBDEB7CA66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED71CCA3-119B-4A47-865E-845A51B50E78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>ssnNumber</t>
   </si>
@@ -84,70 +84,40 @@
     <t>password</t>
   </si>
   <si>
-    <t>Schneider</t>
-  </si>
-  <si>
-    <t>511-434-3547</t>
-  </si>
-  <si>
-    <t>18752</t>
-  </si>
-  <si>
-    <t>19609 Morgan Drive</t>
-  </si>
-  <si>
-    <t>South Ninfaside</t>
-  </si>
-  <si>
-    <t>375-15-7057</t>
-  </si>
-  <si>
-    <t>amanda.rodriguez</t>
-  </si>
-  <si>
-    <t>Wallace</t>
-  </si>
-  <si>
-    <t>cC5;–9Z</t>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>107-834-0930</t>
+  </si>
+  <si>
+    <t>10539-6009</t>
+  </si>
+  <si>
+    <t>526 Gary Cape</t>
+  </si>
+  <si>
+    <t>Ernserhaven</t>
+  </si>
+  <si>
+    <t>738-94-4683</t>
+  </si>
+  <si>
+    <t>al.bradtke</t>
+  </si>
+  <si>
+    <t>Era</t>
+  </si>
+  <si>
+    <t>nQ6,LjR</t>
   </si>
   <si>
     <t>432-131-5405</t>
   </si>
   <si>
-    <t>Mississippi</t>
-  </si>
-  <si>
-    <t>sal.fisher@hotmail.com</t>
-  </si>
-  <si>
-    <t>Mercy</t>
-  </si>
-  <si>
-    <t>Mante</t>
-  </si>
-  <si>
-    <t>30495</t>
-  </si>
-  <si>
-    <t>28037 Gulgowski Shore</t>
-  </si>
-  <si>
-    <t>588-697-5116</t>
-  </si>
-  <si>
-    <t>Darrickshire</t>
-  </si>
-  <si>
-    <t>364-66-8818</t>
-  </si>
-  <si>
-    <t>Maine</t>
-  </si>
-  <si>
-    <t>claudette.jerde</t>
-  </si>
-  <si>
-    <t>sherley.moen@yahoo.com</t>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>omer.gutmann@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -476,7 +446,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
change map key to String
</commit_message>
<xml_diff>
--- a/src/test/resources/CreatedUserInformation.xlsx
+++ b/src/test/resources/CreatedUserInformation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED71CCA3-119B-4A47-865E-845A51B50E78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C76E04-9BA1-4E07-B837-162147407168}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -124,7 +124,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,23 +445,23 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="3.88671875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="28.5546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="3.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -503,7 +502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -551,24 +550,24 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.21875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="5.77734375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -630,23 +629,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
-    <col min="4" max="5" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.21875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="5.77734375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="2.6640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="17" max="18" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="2.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
map string object correction
</commit_message>
<xml_diff>
--- a/src/test/resources/CreatedUserInformation.xlsx
+++ b/src/test/resources/CreatedUserInformation.xlsx
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>ssnNumber</t>
   </si>
@@ -124,6 +124,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,18 +451,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="3.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="3.88671875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -547,7 +548,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A8C0A6-A5D7-4843-BF59-F8CA009F27C6}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
@@ -555,19 +556,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.21875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="5.77734375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -613,6 +614,30 @@
       <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2"/>
+      <c r="K2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -629,23 +654,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="5.21875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="2.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="7.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="18" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
+    <col min="4" max="5" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="5.21875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="5.77734375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="2.6640625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="17" max="18" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
edit page activation try passed
</commit_message>
<xml_diff>
--- a/src/test/resources/CreatedUserInformation.xlsx
+++ b/src/test/resources/CreatedUserInformation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
   <si>
     <t>ssnNumber</t>
   </si>
@@ -548,7 +548,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A8C0A6-A5D7-4843-BF59-F8CA009F27C6}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
@@ -638,6 +638,30 @@
         <v>28</v>
       </c>
       <c r="N2"/>
+    </row>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3"/>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
admin manages users completed
</commit_message>
<xml_diff>
--- a/src/test/resources/CreatedUserInformation.xlsx
+++ b/src/test/resources/CreatedUserInformation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BA1ED2-A149-4EBB-8CC7-42C0264CB051}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF197C8-3EB1-43AC-B55F-8B51AB770071}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="88">
   <si>
     <t>ssnNumber</t>
   </si>
@@ -81,91 +81,211 @@
     <t>password</t>
   </si>
   <si>
-    <t>Cole</t>
+    <t>Corwin</t>
+  </si>
+  <si>
+    <t>206-381-6032</t>
+  </si>
+  <si>
+    <t>3764 Mariah Walk</t>
+  </si>
+  <si>
+    <t>102-86-9325</t>
+  </si>
+  <si>
+    <t>jaime.okeefe</t>
+  </si>
+  <si>
+    <t>Wilmer</t>
+  </si>
+  <si>
+    <t>sF2#KWD</t>
+  </si>
+  <si>
+    <t>elke.kshlerin@hotmail.com</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>ROLE_ADMIN</t>
+  </si>
+  <si>
+    <t>60512</t>
+  </si>
+  <si>
+    <t>O'Hara</t>
+  </si>
+  <si>
+    <t>107-834-0930</t>
+  </si>
+  <si>
+    <t>033 Dooley Isle</t>
+  </si>
+  <si>
+    <t>786-42-1364</t>
+  </si>
+  <si>
+    <t>jan.bergnaum</t>
+  </si>
+  <si>
+    <t>Doug</t>
+  </si>
+  <si>
+    <t>tR5#F:c</t>
+  </si>
+  <si>
+    <t>renaldo.buckridge@hotmail.com</t>
+  </si>
+  <si>
+    <t>60513</t>
+  </si>
+  <si>
+    <t>Frami</t>
+  </si>
+  <si>
+    <t>715-457-6770</t>
+  </si>
+  <si>
+    <t>7066 Dare Lock</t>
+  </si>
+  <si>
+    <t>593-39-9231</t>
+  </si>
+  <si>
+    <t>mao.weber</t>
+  </si>
+  <si>
+    <t>Nickolas</t>
+  </si>
+  <si>
+    <t>gD4@@Q)</t>
+  </si>
+  <si>
+    <t>kristel.harris@gmail.com</t>
+  </si>
+  <si>
+    <t>60514</t>
+  </si>
+  <si>
+    <t>nullguoD</t>
+  </si>
+  <si>
+    <t>Rempel</t>
+  </si>
+  <si>
+    <t>54767-3373</t>
+  </si>
+  <si>
+    <t>3919 Abbott Harbors</t>
+  </si>
+  <si>
+    <t>East Dalton</t>
+  </si>
+  <si>
+    <t>329-73-7753</t>
+  </si>
+  <si>
+    <t>mikki.dickens</t>
+  </si>
+  <si>
+    <t>Ty</t>
+  </si>
+  <si>
+    <t>qX2,69c</t>
+  </si>
+  <si>
+    <t>189-843-0512</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>joycelyn.schuster@yahoo.com</t>
+  </si>
+  <si>
+    <t>60518</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>967-954-5421</t>
+  </si>
+  <si>
+    <t>03600</t>
+  </si>
+  <si>
+    <t>42302 Tabitha Hollow</t>
+  </si>
+  <si>
+    <t>South Elbert</t>
+  </si>
+  <si>
+    <t>621-63-3466</t>
+  </si>
+  <si>
+    <t>natashia.ritchie</t>
+  </si>
+  <si>
+    <t>Jacques</t>
+  </si>
+  <si>
+    <t>eX9+2@t</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>regenia.homenick@yahoo.com</t>
+  </si>
+  <si>
+    <t>ROLE_USER</t>
+  </si>
+  <si>
+    <t>60519</t>
+  </si>
+  <si>
+    <t>Mueller</t>
+  </si>
+  <si>
+    <t>79956</t>
+  </si>
+  <si>
+    <t>498 Harris Alley</t>
+  </si>
+  <si>
+    <t>Bradtkemouth</t>
+  </si>
+  <si>
+    <t>438-52-0014</t>
+  </si>
+  <si>
+    <t>adaline.bednar</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>mY2~3[&gt;</t>
   </si>
   <si>
     <t>588-697-5116</t>
   </si>
   <si>
-    <t>99238</t>
-  </si>
-  <si>
-    <t>24589 Keebler Land</t>
-  </si>
-  <si>
-    <t>North Rosy</t>
-  </si>
-  <si>
-    <t>499-68-6638</t>
-  </si>
-  <si>
-    <t>rema.predovic</t>
-  </si>
-  <si>
-    <t>Travis</t>
-  </si>
-  <si>
-    <t>cK2(&amp;!5</t>
-  </si>
-  <si>
-    <t>206-381-6032</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>harris.white@yahoo.com</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>ROLE_ADMIN</t>
-  </si>
-  <si>
-    <t>60510</t>
-  </si>
-  <si>
-    <t>Conn</t>
-  </si>
-  <si>
-    <t>511-434-3547</t>
-  </si>
-  <si>
-    <t>36415</t>
-  </si>
-  <si>
-    <t>406 Nancee Greens</t>
-  </si>
-  <si>
-    <t>Jameytown</t>
-  </si>
-  <si>
-    <t>004-11-4588</t>
-  </si>
-  <si>
-    <t>pamela.schaefer</t>
-  </si>
-  <si>
-    <t>Roxann</t>
-  </si>
-  <si>
-    <t>gU0~eO^</t>
-  </si>
-  <si>
-    <t>715-457-6770</t>
-  </si>
-  <si>
-    <t>Vermont</t>
-  </si>
-  <si>
-    <t>williemae.mccullough@hotmail.com</t>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>deandre.greenfelder@hotmail.com</t>
   </si>
   <si>
     <t>ROLE_EMPLOYEE</t>
   </si>
   <si>
-    <t>60511</t>
+    <t>60520</t>
+  </si>
+  <si>
+    <t>seuqcaJ</t>
   </si>
 </sst>
 </file>
@@ -494,7 +614,7 @@
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,10 +679,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A8C0A6-A5D7-4843-BF59-F8CA009F27C6}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,82 +737,152 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
+        <v>21</v>
+      </c>
       <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="I2"/>
       <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
         <v>27</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="N2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
+      <c r="I4"/>
+      <c r="J4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3"/>
-      <c r="J3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" t="s">
-        <v>47</v>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add end to end following: registration, database valdiation, api validation, employee sign in
</commit_message>
<xml_diff>
--- a/src/test/resources/CreatedUserInformation.xlsx
+++ b/src/test/resources/CreatedUserInformation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82514313-71AD-418E-BBA6-80EFFE6D7D57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37F7649-9896-4523-834E-A9D02EFBFDAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="161">
   <si>
     <t>ssnNumber</t>
   </si>
@@ -277,6 +277,234 @@
   </si>
   <si>
     <t>60537</t>
+  </si>
+  <si>
+    <t>Jenkins</t>
+  </si>
+  <si>
+    <t>98165</t>
+  </si>
+  <si>
+    <t>98990 Dorian Fort</t>
+  </si>
+  <si>
+    <t>South Maxstad</t>
+  </si>
+  <si>
+    <t>016-03-0850</t>
+  </si>
+  <si>
+    <t>allena.hoppe</t>
+  </si>
+  <si>
+    <t>Hollis</t>
+  </si>
+  <si>
+    <t>oQ6/*;f</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>damaris.okuneva@gmail.com</t>
+  </si>
+  <si>
+    <t>61560</t>
+  </si>
+  <si>
+    <t>Yost</t>
+  </si>
+  <si>
+    <t>94764-5210</t>
+  </si>
+  <si>
+    <t>752 Feeney Orchard</t>
+  </si>
+  <si>
+    <t>South Janview</t>
+  </si>
+  <si>
+    <t>286-43-1531</t>
+  </si>
+  <si>
+    <t>esta.connelly</t>
+  </si>
+  <si>
+    <t>kS3)*=J</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>sean.aufderhar@gmail.com</t>
+  </si>
+  <si>
+    <t>61561</t>
+  </si>
+  <si>
+    <t>niboR</t>
+  </si>
+  <si>
+    <t>Batz</t>
+  </si>
+  <si>
+    <t>21647-8744</t>
+  </si>
+  <si>
+    <t>080 Maranda Hills</t>
+  </si>
+  <si>
+    <t>Phuongton</t>
+  </si>
+  <si>
+    <t>397-14-9798</t>
+  </si>
+  <si>
+    <t>dalene.dicki</t>
+  </si>
+  <si>
+    <t>Arla</t>
+  </si>
+  <si>
+    <t>qX7}I!0</t>
+  </si>
+  <si>
+    <t>107-834-0930</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>akilah.beahan@hotmail.com</t>
+  </si>
+  <si>
+    <t>Brakus</t>
+  </si>
+  <si>
+    <t>85577-0223</t>
+  </si>
+  <si>
+    <t>57174 Paucek Forge</t>
+  </si>
+  <si>
+    <t>Port Sherikaborough</t>
+  </si>
+  <si>
+    <t>479-87-8631</t>
+  </si>
+  <si>
+    <t>harold.zulauf</t>
+  </si>
+  <si>
+    <t>Chester</t>
+  </si>
+  <si>
+    <t>eS9:OJz</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>neely.cummings@gmail.com</t>
+  </si>
+  <si>
+    <t>Ankunding</t>
+  </si>
+  <si>
+    <t>98336</t>
+  </si>
+  <si>
+    <t>391 Fritsch Manor</t>
+  </si>
+  <si>
+    <t>Manntown</t>
+  </si>
+  <si>
+    <t>781-99-3691</t>
+  </si>
+  <si>
+    <t>jeromy.dooley</t>
+  </si>
+  <si>
+    <t>Edgar</t>
+  </si>
+  <si>
+    <t>aD1&lt;5/F</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>minh.bednar@hotmail.com</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Strosin</t>
+  </si>
+  <si>
+    <t>09652</t>
+  </si>
+  <si>
+    <t>86776 Lonnie Drives</t>
+  </si>
+  <si>
+    <t>Muellerhaven</t>
+  </si>
+  <si>
+    <t>172-83-7736</t>
+  </si>
+  <si>
+    <t>nguyet.welch</t>
+  </si>
+  <si>
+    <t>Todd</t>
+  </si>
+  <si>
+    <t>nZ4&lt;vj/</t>
+  </si>
+  <si>
+    <t>319-959-3517</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>johnson.reichert@hotmail.com</t>
+  </si>
+  <si>
+    <t>Carter</t>
+  </si>
+  <si>
+    <t>206-381-6032</t>
+  </si>
+  <si>
+    <t>74028</t>
+  </si>
+  <si>
+    <t>807 Frederic Mount</t>
+  </si>
+  <si>
+    <t>Luisefurt</t>
+  </si>
+  <si>
+    <t>432-56-6151</t>
+  </si>
+  <si>
+    <t>maurice.labadie</t>
+  </si>
+  <si>
+    <t>Jospeh</t>
+  </si>
+  <si>
+    <t>rA2!?tm</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>li.hagenes@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -602,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,7 +852,7 @@
     <col min="12" max="12" bestFit="true" customWidth="true" width="12.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,6 +888,199 @@
       </c>
       <c r="L1" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K2" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>123</v>
+      </c>
+      <c r="K3" t="s">
+        <v>127</v>
+      </c>
+      <c r="L3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K4" t="s">
+        <v>137</v>
+      </c>
+      <c r="L4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" t="s">
+        <v>147</v>
+      </c>
+      <c r="J5" t="s">
+        <v>144</v>
+      </c>
+      <c r="K5" t="s">
+        <v>149</v>
+      </c>
+      <c r="L5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" t="s">
+        <v>151</v>
+      </c>
+      <c r="I6" t="s">
+        <v>147</v>
+      </c>
+      <c r="J6" t="s">
+        <v>156</v>
+      </c>
+      <c r="K6" t="s">
+        <v>160</v>
+      </c>
+      <c r="L6" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -670,18 +1091,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A8C0A6-A5D7-4843-BF59-F8CA009F27C6}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F5" sqref="A5:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="15" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="1" max="5" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="7" max="16" customWidth="true" width="22.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -698,37 +1121,40 @@
         <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -741,29 +1167,29 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>27</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>28</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>29</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -776,29 +1202,29 @@
       <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>35</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>38</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>37</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>28</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>39</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -811,29 +1237,29 @@
       <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>44</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>47</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>46</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>28</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>48</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -849,36 +1275,35 @@
       <c r="E5" t="s">
         <v>52</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>54</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>59</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>51</v>
       </c>
-      <c r="I5"/>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>56</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>60</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>58</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>28</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>29</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -894,36 +1319,35 @@
       <c r="E6" t="s">
         <v>63</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>65</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>71</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>26</v>
       </c>
-      <c r="I6"/>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>67</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>72</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>69</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>28</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>39</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -939,33 +1363,120 @@
       <c r="E7" t="s">
         <v>75</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>77</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>82</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>32</v>
       </c>
-      <c r="I7"/>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>79</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>83</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>81</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>28</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>48</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" t="s">
+        <v>88</v>
+      </c>
+      <c r="H8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" t="s">
+        <v>90</v>
+      </c>
+      <c r="L8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M8" t="s">
+        <v>92</v>
+      </c>
+      <c r="N8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G9" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" t="s">
+        <v>103</v>
+      </c>
+      <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" t="s">
+        <v>101</v>
+      </c>
+      <c r="L9" t="s">
+        <v>104</v>
+      </c>
+      <c r="M9" t="s">
+        <v>102</v>
+      </c>
+      <c r="N9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" t="s">
+        <v>39</v>
+      </c>
+      <c r="P9" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -975,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55BFD007-6D85-4BB6-B9BF-B15426A563F8}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:R1048576"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -988,21 +1499,22 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.109375" collapsed="true"/>
     <col min="4" max="5" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="4.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="5.21875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="5.77734375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="2.6640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="17" max="18" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="4.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="5.21875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="5.77734375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="2.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="18" max="19" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1022,42 +1534,45 @@
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
end to end till API, missing mapfromUI
</commit_message>
<xml_diff>
--- a/src/test/resources/CreatedUserInformation.xlsx
+++ b/src/test/resources/CreatedUserInformation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="210">
   <si>
     <t>ssnNumber</t>
   </si>
@@ -505,6 +505,153 @@
   </si>
   <si>
     <t>li.hagenes@yahoo.com</t>
+  </si>
+  <si>
+    <t>Borer</t>
+  </si>
+  <si>
+    <t>98552</t>
+  </si>
+  <si>
+    <t>89746 Keeling Wall</t>
+  </si>
+  <si>
+    <t>Lake Edgardo</t>
+  </si>
+  <si>
+    <t>434-46-9744</t>
+  </si>
+  <si>
+    <t>ervin.treutel</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>tX5#&lt;qp</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>juan.fay@hotmail.com</t>
+  </si>
+  <si>
+    <t>Weimann</t>
+  </si>
+  <si>
+    <t>34974-5909</t>
+  </si>
+  <si>
+    <t>8445 Farrell Unions</t>
+  </si>
+  <si>
+    <t>Bradlyfort</t>
+  </si>
+  <si>
+    <t>497-09-8615</t>
+  </si>
+  <si>
+    <t>tonisha.kutch</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>hW0+q/g</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>king.casper@yahoo.com</t>
+  </si>
+  <si>
+    <t>O'Reilly</t>
+  </si>
+  <si>
+    <t>89051</t>
+  </si>
+  <si>
+    <t>52535 Allan Square</t>
+  </si>
+  <si>
+    <t>Barrowsmouth</t>
+  </si>
+  <si>
+    <t>292-81-6208</t>
+  </si>
+  <si>
+    <t>leesa.maggio</t>
+  </si>
+  <si>
+    <t>Kellye</t>
+  </si>
+  <si>
+    <t>kV0(V&lt;V</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>joan.kessler@hotmail.com</t>
+  </si>
+  <si>
+    <t>Raynor</t>
+  </si>
+  <si>
+    <t>46114</t>
+  </si>
+  <si>
+    <t>374 Jakubowski Grove</t>
+  </si>
+  <si>
+    <t>Shalandaland</t>
+  </si>
+  <si>
+    <t>141-83-0402</t>
+  </si>
+  <si>
+    <t>johnetta.nolan</t>
+  </si>
+  <si>
+    <t>Darwin</t>
+  </si>
+  <si>
+    <t>eB8,{/w</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>lupe.balistreri@hotmail.com</t>
+  </si>
+  <si>
+    <t>Greenholt</t>
+  </si>
+  <si>
+    <t>47676</t>
+  </si>
+  <si>
+    <t>23742 Michale Islands</t>
+  </si>
+  <si>
+    <t>Lake Mariettabury</t>
+  </si>
+  <si>
+    <t>553-25-2381</t>
+  </si>
+  <si>
+    <t>lindsay.morissette</t>
+  </si>
+  <si>
+    <t>Hertha</t>
+  </si>
+  <si>
+    <t>kW2^:O$</t>
+  </si>
+  <si>
+    <t>kelly.dach@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -830,7 +977,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
@@ -1081,6 +1228,196 @@
       </c>
       <c r="L6" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" t="s">
+        <v>164</v>
+      </c>
+      <c r="G7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" t="s">
+        <v>115</v>
+      </c>
+      <c r="J7" t="s">
+        <v>166</v>
+      </c>
+      <c r="K7" t="s">
+        <v>170</v>
+      </c>
+      <c r="L7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D8" t="s">
+        <v>173</v>
+      </c>
+      <c r="E8" t="s">
+        <v>172</v>
+      </c>
+      <c r="F8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G8" t="s">
+        <v>179</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
+        <v>176</v>
+      </c>
+      <c r="K8" t="s">
+        <v>180</v>
+      </c>
+      <c r="L8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" t="s">
+        <v>184</v>
+      </c>
+      <c r="G9" t="s">
+        <v>189</v>
+      </c>
+      <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" t="s">
+        <v>186</v>
+      </c>
+      <c r="K9" t="s">
+        <v>190</v>
+      </c>
+      <c r="L9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" t="s">
+        <v>193</v>
+      </c>
+      <c r="E10" t="s">
+        <v>192</v>
+      </c>
+      <c r="F10" t="s">
+        <v>194</v>
+      </c>
+      <c r="G10" t="s">
+        <v>199</v>
+      </c>
+      <c r="H10" t="s">
+        <v>151</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>196</v>
+      </c>
+      <c r="K10" t="s">
+        <v>200</v>
+      </c>
+      <c r="L10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D11" t="s">
+        <v>203</v>
+      </c>
+      <c r="E11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F11" t="s">
+        <v>204</v>
+      </c>
+      <c r="G11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>147</v>
+      </c>
+      <c r="J11" t="s">
+        <v>206</v>
+      </c>
+      <c r="K11" t="s">
+        <v>209</v>
+      </c>
+      <c r="L11" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
customer creation end to end test
</commit_message>
<xml_diff>
--- a/src/test/resources/CreatedUserInformation.xlsx
+++ b/src/test/resources/CreatedUserInformation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="452">
   <si>
     <t>ssnNumber</t>
   </si>
@@ -652,6 +652,732 @@
   </si>
   <si>
     <t>kelly.dach@hotmail.com</t>
+  </si>
+  <si>
+    <t>Bartell</t>
+  </si>
+  <si>
+    <t>01532</t>
+  </si>
+  <si>
+    <t>293 Rufus Extensions</t>
+  </si>
+  <si>
+    <t>Swaniawskiside</t>
+  </si>
+  <si>
+    <t>898-74-5291</t>
+  </si>
+  <si>
+    <t>marianela.funk</t>
+  </si>
+  <si>
+    <t>Hang</t>
+  </si>
+  <si>
+    <t>uG2#I/^</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>nicolas.zemlak@yahoo.com</t>
+  </si>
+  <si>
+    <t>Kemmer</t>
+  </si>
+  <si>
+    <t>22601-3800</t>
+  </si>
+  <si>
+    <t>7197 Thiel Well</t>
+  </si>
+  <si>
+    <t>New Ashantifurt</t>
+  </si>
+  <si>
+    <t>309-75-3963</t>
+  </si>
+  <si>
+    <t>sigrid.hamill</t>
+  </si>
+  <si>
+    <t>Maryellen</t>
+  </si>
+  <si>
+    <t>eI6&amp;7TB</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>cordia.corkery@gmail.com</t>
+  </si>
+  <si>
+    <t>Steuber</t>
+  </si>
+  <si>
+    <t>14384</t>
+  </si>
+  <si>
+    <t>710 Rosanna Drive</t>
+  </si>
+  <si>
+    <t>North Nedra</t>
+  </si>
+  <si>
+    <t>836-33-2977</t>
+  </si>
+  <si>
+    <t>daren.cormier</t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
+    <t>hW9–KAZ</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>eloy.stokes@yahoo.com</t>
+  </si>
+  <si>
+    <t>Lowe</t>
+  </si>
+  <si>
+    <t>54470-5132</t>
+  </si>
+  <si>
+    <t>53389 Barton Orchard</t>
+  </si>
+  <si>
+    <t>Strosinland</t>
+  </si>
+  <si>
+    <t>754-05-5895</t>
+  </si>
+  <si>
+    <t>haley.treutel</t>
+  </si>
+  <si>
+    <t>Randi</t>
+  </si>
+  <si>
+    <t>dJ3(KUV</t>
+  </si>
+  <si>
+    <t>715-457-6770</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>lupe.funk@yahoo.com</t>
+  </si>
+  <si>
+    <t>Waelchi</t>
+  </si>
+  <si>
+    <t>38071</t>
+  </si>
+  <si>
+    <t>0984 Haley Keys</t>
+  </si>
+  <si>
+    <t>West Jewell</t>
+  </si>
+  <si>
+    <t>802-92-2872</t>
+  </si>
+  <si>
+    <t>kendall.labadie</t>
+  </si>
+  <si>
+    <t>Lelah</t>
+  </si>
+  <si>
+    <t>gI0{n?*</t>
+  </si>
+  <si>
+    <t>julio.connelly@gmail.com</t>
+  </si>
+  <si>
+    <t>Schmidt</t>
+  </si>
+  <si>
+    <t>02909-4324</t>
+  </si>
+  <si>
+    <t>1810 Anisa Street</t>
+  </si>
+  <si>
+    <t>Kuhicview</t>
+  </si>
+  <si>
+    <t>357-68-1614</t>
+  </si>
+  <si>
+    <t>herbert.harris</t>
+  </si>
+  <si>
+    <t>Asa</t>
+  </si>
+  <si>
+    <t>tM3=&lt;&gt;(</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>rich.erdman@hotmail.com</t>
+  </si>
+  <si>
+    <t>Pacocha</t>
+  </si>
+  <si>
+    <t>99297</t>
+  </si>
+  <si>
+    <t>696 Nickolas Place</t>
+  </si>
+  <si>
+    <t>Devonburgh</t>
+  </si>
+  <si>
+    <t>325-06-9910</t>
+  </si>
+  <si>
+    <t>wesley.wiegand</t>
+  </si>
+  <si>
+    <t>Amber</t>
+  </si>
+  <si>
+    <t>aR5[8LL</t>
+  </si>
+  <si>
+    <t>randy.hoppe@hotmail.com</t>
+  </si>
+  <si>
+    <t>Harber</t>
+  </si>
+  <si>
+    <t>03351-0751</t>
+  </si>
+  <si>
+    <t>44609 Kuvalis Crossing</t>
+  </si>
+  <si>
+    <t>Valorieland</t>
+  </si>
+  <si>
+    <t>609-80-4637</t>
+  </si>
+  <si>
+    <t>michal.kohler</t>
+  </si>
+  <si>
+    <t>Corene</t>
+  </si>
+  <si>
+    <t>xN0#S5v</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>moses.satterfield@hotmail.com</t>
+  </si>
+  <si>
+    <t>Heller</t>
+  </si>
+  <si>
+    <t>03137-3518</t>
+  </si>
+  <si>
+    <t>02048 Prosacco Highway</t>
+  </si>
+  <si>
+    <t>Port Garretmouth</t>
+  </si>
+  <si>
+    <t>851-01-8508</t>
+  </si>
+  <si>
+    <t>lillia.dickens</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>eB9(gcS</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>carey.monahan@hotmail.com</t>
+  </si>
+  <si>
+    <t>Becker</t>
+  </si>
+  <si>
+    <t>69586</t>
+  </si>
+  <si>
+    <t>38589 Landon Forest</t>
+  </si>
+  <si>
+    <t>Rickyburgh</t>
+  </si>
+  <si>
+    <t>034-90-3565</t>
+  </si>
+  <si>
+    <t>josef.gibson</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>hA0&gt;5/f</t>
+  </si>
+  <si>
+    <t>cleopatra.steuber@gmail.com</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>55097-9016</t>
+  </si>
+  <si>
+    <t>72337 Robert Trail</t>
+  </si>
+  <si>
+    <t>Lake Chantaymouth</t>
+  </si>
+  <si>
+    <t>336-17-2430</t>
+  </si>
+  <si>
+    <t>vonda.schmidt</t>
+  </si>
+  <si>
+    <t>Suzy</t>
+  </si>
+  <si>
+    <t>iB7/Ura</t>
+  </si>
+  <si>
+    <t>farrah.mante@gmail.com</t>
+  </si>
+  <si>
+    <t>Considine</t>
+  </si>
+  <si>
+    <t>74219-0957</t>
+  </si>
+  <si>
+    <t>402 Goldner Squares</t>
+  </si>
+  <si>
+    <t>East Allenfurt</t>
+  </si>
+  <si>
+    <t>054-41-1762</t>
+  </si>
+  <si>
+    <t>debbra.effertz</t>
+  </si>
+  <si>
+    <t>Marc</t>
+  </si>
+  <si>
+    <t>mE6}7bM</t>
+  </si>
+  <si>
+    <t>cyndi.windler@hotmail.com</t>
+  </si>
+  <si>
+    <t>Kuhic</t>
+  </si>
+  <si>
+    <t>33194-4593</t>
+  </si>
+  <si>
+    <t>1976 Gino Mall</t>
+  </si>
+  <si>
+    <t>West Randa</t>
+  </si>
+  <si>
+    <t>709-81-8304</t>
+  </si>
+  <si>
+    <t>lashon.macgyver</t>
+  </si>
+  <si>
+    <t>Herta</t>
+  </si>
+  <si>
+    <t>iB7)v^&lt;</t>
+  </si>
+  <si>
+    <t>ellis.bernier@hotmail.com</t>
+  </si>
+  <si>
+    <t>Maggio</t>
+  </si>
+  <si>
+    <t>08340</t>
+  </si>
+  <si>
+    <t>2028 Parker Forges</t>
+  </si>
+  <si>
+    <t>Lake Jordon</t>
+  </si>
+  <si>
+    <t>057-63-8250</t>
+  </si>
+  <si>
+    <t>reid.klocko</t>
+  </si>
+  <si>
+    <t>Logan</t>
+  </si>
+  <si>
+    <t>wU4–;w!</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>octavio.zboncak@gmail.com</t>
+  </si>
+  <si>
+    <t>Tillman</t>
+  </si>
+  <si>
+    <t>46930-6203</t>
+  </si>
+  <si>
+    <t>076 Melvina Junctions</t>
+  </si>
+  <si>
+    <t>North Quinn</t>
+  </si>
+  <si>
+    <t>859-83-4387</t>
+  </si>
+  <si>
+    <t>andrea.farrell</t>
+  </si>
+  <si>
+    <t>Raisa</t>
+  </si>
+  <si>
+    <t>sV8?2x8</t>
+  </si>
+  <si>
+    <t>reagan.dach@yahoo.com</t>
+  </si>
+  <si>
+    <t>Morar</t>
+  </si>
+  <si>
+    <t>60521-6401</t>
+  </si>
+  <si>
+    <t>861 Clifford Highway</t>
+  </si>
+  <si>
+    <t>North Youlanda</t>
+  </si>
+  <si>
+    <t>825-87-7524</t>
+  </si>
+  <si>
+    <t>lexie.heaney</t>
+  </si>
+  <si>
+    <t>Lon</t>
+  </si>
+  <si>
+    <t>lG2&gt;v(~</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>reuben.vandervort@gmail.com</t>
+  </si>
+  <si>
+    <t>Rogahn</t>
+  </si>
+  <si>
+    <t>81643</t>
+  </si>
+  <si>
+    <t>8387 Rosenbaum Shoal</t>
+  </si>
+  <si>
+    <t>Mosciskimouth</t>
+  </si>
+  <si>
+    <t>372-74-8288</t>
+  </si>
+  <si>
+    <t>marilyn.hegmann</t>
+  </si>
+  <si>
+    <t>Reyes</t>
+  </si>
+  <si>
+    <t>pG5}yrS</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>raphael.purdy@yahoo.com</t>
+  </si>
+  <si>
+    <t>61924</t>
+  </si>
+  <si>
+    <t>231 Wunsch Brooks</t>
+  </si>
+  <si>
+    <t>East Chrisport</t>
+  </si>
+  <si>
+    <t>232-78-3042</t>
+  </si>
+  <si>
+    <t>omega.terry</t>
+  </si>
+  <si>
+    <t>Kerry</t>
+  </si>
+  <si>
+    <t>lJ4&amp;c6?</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>matthew.boehm@yahoo.com</t>
+  </si>
+  <si>
+    <t>Bartoletti</t>
+  </si>
+  <si>
+    <t>20670-7308</t>
+  </si>
+  <si>
+    <t>3188 Beverley Ford</t>
+  </si>
+  <si>
+    <t>New Aubrey</t>
+  </si>
+  <si>
+    <t>304-63-9260</t>
+  </si>
+  <si>
+    <t>jed.glover</t>
+  </si>
+  <si>
+    <t>Nolan</t>
+  </si>
+  <si>
+    <t>qL8–Em)</t>
+  </si>
+  <si>
+    <t>tillie.aufderhar@gmail.com</t>
+  </si>
+  <si>
+    <t>Daugherty</t>
+  </si>
+  <si>
+    <t>54061</t>
+  </si>
+  <si>
+    <t>5938 Treutel Grove</t>
+  </si>
+  <si>
+    <t>Lindview</t>
+  </si>
+  <si>
+    <t>500-26-8147</t>
+  </si>
+  <si>
+    <t>noelle.predovic</t>
+  </si>
+  <si>
+    <t>Marty</t>
+  </si>
+  <si>
+    <t>zZ7&lt;B{S</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>shaunna.schmitt@yahoo.com</t>
+  </si>
+  <si>
+    <t>72758</t>
+  </si>
+  <si>
+    <t>85879 Kovacek Roads</t>
+  </si>
+  <si>
+    <t>Anniechester</t>
+  </si>
+  <si>
+    <t>621-08-6725</t>
+  </si>
+  <si>
+    <t>christine.vonrueden</t>
+  </si>
+  <si>
+    <t>Lilly</t>
+  </si>
+  <si>
+    <t>bN6=ahw</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>paris.nienow@gmail.com</t>
+  </si>
+  <si>
+    <t>Emmerich</t>
+  </si>
+  <si>
+    <t>30643-4275</t>
+  </si>
+  <si>
+    <t>7320 Jenelle Plaza</t>
+  </si>
+  <si>
+    <t>Turnerfurt</t>
+  </si>
+  <si>
+    <t>490-65-9976</t>
+  </si>
+  <si>
+    <t>erwin.lueilwitz</t>
+  </si>
+  <si>
+    <t>Ariel</t>
+  </si>
+  <si>
+    <t>sU2=ZNa</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>hugh.dare@hotmail.com</t>
+  </si>
+  <si>
+    <t>DuBuque</t>
+  </si>
+  <si>
+    <t>06206</t>
+  </si>
+  <si>
+    <t>70675 Jacquelin Fields</t>
+  </si>
+  <si>
+    <t>West Kelsieborough</t>
+  </si>
+  <si>
+    <t>201-11-9899</t>
+  </si>
+  <si>
+    <t>hang.crooks</t>
+  </si>
+  <si>
+    <t>Majorie</t>
+  </si>
+  <si>
+    <t>nW4(nqC</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>lilla.fritsch@hotmail.com</t>
+  </si>
+  <si>
+    <t>Quitzon</t>
+  </si>
+  <si>
+    <t>39751</t>
+  </si>
+  <si>
+    <t>91161 Lashaunda Square</t>
+  </si>
+  <si>
+    <t>Lake Pearlestad</t>
+  </si>
+  <si>
+    <t>281-06-0169</t>
+  </si>
+  <si>
+    <t>tad.donnelly</t>
+  </si>
+  <si>
+    <t>Matilda</t>
+  </si>
+  <si>
+    <t>dY1!k7H</t>
+  </si>
+  <si>
+    <t>evelin.smith@hotmail.com</t>
+  </si>
+  <si>
+    <t>Reichel</t>
+  </si>
+  <si>
+    <t>15757-3265</t>
+  </si>
+  <si>
+    <t>0495 Hilario Shores</t>
+  </si>
+  <si>
+    <t>Lake Enochland</t>
+  </si>
+  <si>
+    <t>584-05-9172</t>
+  </si>
+  <si>
+    <t>tommie.ritchie</t>
+  </si>
+  <si>
+    <t>Lewis</t>
+  </si>
+  <si>
+    <t>wA1;U;i</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>jesusa.tillman@yahoo.com</t>
+  </si>
+  <si>
+    <t>ROLE_CUSTOMER</t>
+  </si>
+  <si>
+    <t>63465</t>
   </si>
 </sst>
 </file>
@@ -977,7 +1703,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M1" sqref="M1"/>
@@ -1420,6 +2146,880 @@
         <v>208</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D12" t="s">
+        <v>212</v>
+      </c>
+      <c r="E12" t="s">
+        <v>211</v>
+      </c>
+      <c r="F12" t="s">
+        <v>213</v>
+      </c>
+      <c r="G12" t="s">
+        <v>218</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" t="s">
+        <v>215</v>
+      </c>
+      <c r="K12" t="s">
+        <v>219</v>
+      </c>
+      <c r="L12" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E13" t="s">
+        <v>221</v>
+      </c>
+      <c r="F13" t="s">
+        <v>223</v>
+      </c>
+      <c r="G13" t="s">
+        <v>228</v>
+      </c>
+      <c r="H13" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" t="s">
+        <v>225</v>
+      </c>
+      <c r="K13" t="s">
+        <v>229</v>
+      </c>
+      <c r="L13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>234</v>
+      </c>
+      <c r="B14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" t="s">
+        <v>230</v>
+      </c>
+      <c r="D14" t="s">
+        <v>232</v>
+      </c>
+      <c r="E14" t="s">
+        <v>231</v>
+      </c>
+      <c r="F14" t="s">
+        <v>233</v>
+      </c>
+      <c r="G14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H14" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" t="s">
+        <v>147</v>
+      </c>
+      <c r="J14" t="s">
+        <v>235</v>
+      </c>
+      <c r="K14" t="s">
+        <v>239</v>
+      </c>
+      <c r="L14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>244</v>
+      </c>
+      <c r="B15" t="s">
+        <v>246</v>
+      </c>
+      <c r="C15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D15" t="s">
+        <v>242</v>
+      </c>
+      <c r="E15" t="s">
+        <v>241</v>
+      </c>
+      <c r="F15" t="s">
+        <v>243</v>
+      </c>
+      <c r="G15" t="s">
+        <v>249</v>
+      </c>
+      <c r="H15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" t="s">
+        <v>248</v>
+      </c>
+      <c r="J15" t="s">
+        <v>245</v>
+      </c>
+      <c r="K15" t="s">
+        <v>250</v>
+      </c>
+      <c r="L15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>255</v>
+      </c>
+      <c r="B16" t="s">
+        <v>257</v>
+      </c>
+      <c r="C16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16" t="s">
+        <v>253</v>
+      </c>
+      <c r="E16" t="s">
+        <v>252</v>
+      </c>
+      <c r="F16" t="s">
+        <v>254</v>
+      </c>
+      <c r="G16" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" t="s">
+        <v>26</v>
+      </c>
+      <c r="J16" t="s">
+        <v>256</v>
+      </c>
+      <c r="K16" t="s">
+        <v>259</v>
+      </c>
+      <c r="L16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>264</v>
+      </c>
+      <c r="B17" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" t="s">
+        <v>260</v>
+      </c>
+      <c r="D17" t="s">
+        <v>262</v>
+      </c>
+      <c r="E17" t="s">
+        <v>261</v>
+      </c>
+      <c r="F17" t="s">
+        <v>263</v>
+      </c>
+      <c r="G17" t="s">
+        <v>268</v>
+      </c>
+      <c r="H17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" t="s">
+        <v>265</v>
+      </c>
+      <c r="K17" t="s">
+        <v>269</v>
+      </c>
+      <c r="L17" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>274</v>
+      </c>
+      <c r="B18" t="s">
+        <v>276</v>
+      </c>
+      <c r="C18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D18" t="s">
+        <v>272</v>
+      </c>
+      <c r="E18" t="s">
+        <v>271</v>
+      </c>
+      <c r="F18" t="s">
+        <v>273</v>
+      </c>
+      <c r="G18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" t="s">
+        <v>275</v>
+      </c>
+      <c r="K18" t="s">
+        <v>278</v>
+      </c>
+      <c r="L18" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>283</v>
+      </c>
+      <c r="B19" t="s">
+        <v>285</v>
+      </c>
+      <c r="C19" t="s">
+        <v>279</v>
+      </c>
+      <c r="D19" t="s">
+        <v>281</v>
+      </c>
+      <c r="E19" t="s">
+        <v>280</v>
+      </c>
+      <c r="F19" t="s">
+        <v>282</v>
+      </c>
+      <c r="G19" t="s">
+        <v>287</v>
+      </c>
+      <c r="H19" t="s">
+        <v>248</v>
+      </c>
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" t="s">
+        <v>284</v>
+      </c>
+      <c r="K19" t="s">
+        <v>288</v>
+      </c>
+      <c r="L19" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>293</v>
+      </c>
+      <c r="B20" t="s">
+        <v>295</v>
+      </c>
+      <c r="C20" t="s">
+        <v>289</v>
+      </c>
+      <c r="D20" t="s">
+        <v>291</v>
+      </c>
+      <c r="E20" t="s">
+        <v>290</v>
+      </c>
+      <c r="F20" t="s">
+        <v>292</v>
+      </c>
+      <c r="G20" t="s">
+        <v>297</v>
+      </c>
+      <c r="H20" t="s">
+        <v>115</v>
+      </c>
+      <c r="I20" t="s">
+        <v>115</v>
+      </c>
+      <c r="J20" t="s">
+        <v>294</v>
+      </c>
+      <c r="K20" t="s">
+        <v>298</v>
+      </c>
+      <c r="L20" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>303</v>
+      </c>
+      <c r="B21" t="s">
+        <v>305</v>
+      </c>
+      <c r="C21" t="s">
+        <v>299</v>
+      </c>
+      <c r="D21" t="s">
+        <v>301</v>
+      </c>
+      <c r="E21" t="s">
+        <v>300</v>
+      </c>
+      <c r="F21" t="s">
+        <v>302</v>
+      </c>
+      <c r="G21" t="s">
+        <v>189</v>
+      </c>
+      <c r="H21" t="s">
+        <v>147</v>
+      </c>
+      <c r="I21" t="s">
+        <v>115</v>
+      </c>
+      <c r="J21" t="s">
+        <v>304</v>
+      </c>
+      <c r="K21" t="s">
+        <v>307</v>
+      </c>
+      <c r="L21" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>312</v>
+      </c>
+      <c r="B22" t="s">
+        <v>314</v>
+      </c>
+      <c r="C22" t="s">
+        <v>308</v>
+      </c>
+      <c r="D22" t="s">
+        <v>310</v>
+      </c>
+      <c r="E22" t="s">
+        <v>309</v>
+      </c>
+      <c r="F22" t="s">
+        <v>311</v>
+      </c>
+      <c r="G22" t="s">
+        <v>238</v>
+      </c>
+      <c r="H22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" t="s">
+        <v>147</v>
+      </c>
+      <c r="J22" t="s">
+        <v>313</v>
+      </c>
+      <c r="K22" t="s">
+        <v>316</v>
+      </c>
+      <c r="L22" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>321</v>
+      </c>
+      <c r="B23" t="s">
+        <v>323</v>
+      </c>
+      <c r="C23" t="s">
+        <v>317</v>
+      </c>
+      <c r="D23" t="s">
+        <v>319</v>
+      </c>
+      <c r="E23" t="s">
+        <v>318</v>
+      </c>
+      <c r="F23" t="s">
+        <v>320</v>
+      </c>
+      <c r="G23" t="s">
+        <v>228</v>
+      </c>
+      <c r="H23" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" t="s">
+        <v>322</v>
+      </c>
+      <c r="K23" t="s">
+        <v>325</v>
+      </c>
+      <c r="L23" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>330</v>
+      </c>
+      <c r="B24" t="s">
+        <v>332</v>
+      </c>
+      <c r="C24" t="s">
+        <v>326</v>
+      </c>
+      <c r="D24" t="s">
+        <v>328</v>
+      </c>
+      <c r="E24" t="s">
+        <v>327</v>
+      </c>
+      <c r="F24" t="s">
+        <v>329</v>
+      </c>
+      <c r="G24" t="s">
+        <v>249</v>
+      </c>
+      <c r="H24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I24" t="s">
+        <v>147</v>
+      </c>
+      <c r="J24" t="s">
+        <v>331</v>
+      </c>
+      <c r="K24" t="s">
+        <v>334</v>
+      </c>
+      <c r="L24" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>339</v>
+      </c>
+      <c r="B25" t="s">
+        <v>341</v>
+      </c>
+      <c r="C25" t="s">
+        <v>335</v>
+      </c>
+      <c r="D25" t="s">
+        <v>337</v>
+      </c>
+      <c r="E25" t="s">
+        <v>336</v>
+      </c>
+      <c r="F25" t="s">
+        <v>338</v>
+      </c>
+      <c r="G25" t="s">
+        <v>343</v>
+      </c>
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" t="s">
+        <v>248</v>
+      </c>
+      <c r="J25" t="s">
+        <v>340</v>
+      </c>
+      <c r="K25" t="s">
+        <v>344</v>
+      </c>
+      <c r="L25" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>349</v>
+      </c>
+      <c r="B26" t="s">
+        <v>351</v>
+      </c>
+      <c r="C26" t="s">
+        <v>345</v>
+      </c>
+      <c r="D26" t="s">
+        <v>347</v>
+      </c>
+      <c r="E26" t="s">
+        <v>346</v>
+      </c>
+      <c r="F26" t="s">
+        <v>348</v>
+      </c>
+      <c r="G26" t="s">
+        <v>249</v>
+      </c>
+      <c r="H26" t="s">
+        <v>151</v>
+      </c>
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s">
+        <v>350</v>
+      </c>
+      <c r="K26" t="s">
+        <v>353</v>
+      </c>
+      <c r="L26" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>358</v>
+      </c>
+      <c r="B27" t="s">
+        <v>360</v>
+      </c>
+      <c r="C27" t="s">
+        <v>354</v>
+      </c>
+      <c r="D27" t="s">
+        <v>356</v>
+      </c>
+      <c r="E27" t="s">
+        <v>355</v>
+      </c>
+      <c r="F27" t="s">
+        <v>357</v>
+      </c>
+      <c r="G27" t="s">
+        <v>362</v>
+      </c>
+      <c r="H27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" t="s">
+        <v>359</v>
+      </c>
+      <c r="K27" t="s">
+        <v>363</v>
+      </c>
+      <c r="L27" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>368</v>
+      </c>
+      <c r="B28" t="s">
+        <v>370</v>
+      </c>
+      <c r="C28" t="s">
+        <v>364</v>
+      </c>
+      <c r="D28" t="s">
+        <v>366</v>
+      </c>
+      <c r="E28" t="s">
+        <v>365</v>
+      </c>
+      <c r="F28" t="s">
+        <v>367</v>
+      </c>
+      <c r="G28" t="s">
+        <v>372</v>
+      </c>
+      <c r="H28" t="s">
+        <v>151</v>
+      </c>
+      <c r="I28" t="s">
+        <v>20</v>
+      </c>
+      <c r="J28" t="s">
+        <v>369</v>
+      </c>
+      <c r="K28" t="s">
+        <v>373</v>
+      </c>
+      <c r="L28" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>377</v>
+      </c>
+      <c r="B29" t="s">
+        <v>379</v>
+      </c>
+      <c r="C29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>375</v>
+      </c>
+      <c r="E29" t="s">
+        <v>374</v>
+      </c>
+      <c r="F29" t="s">
+        <v>376</v>
+      </c>
+      <c r="G29" t="s">
+        <v>381</v>
+      </c>
+      <c r="H29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" t="s">
+        <v>378</v>
+      </c>
+      <c r="K29" t="s">
+        <v>382</v>
+      </c>
+      <c r="L29" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>387</v>
+      </c>
+      <c r="B30" t="s">
+        <v>389</v>
+      </c>
+      <c r="C30" t="s">
+        <v>383</v>
+      </c>
+      <c r="D30" t="s">
+        <v>385</v>
+      </c>
+      <c r="E30" t="s">
+        <v>384</v>
+      </c>
+      <c r="F30" t="s">
+        <v>386</v>
+      </c>
+      <c r="G30" t="s">
+        <v>179</v>
+      </c>
+      <c r="H30" t="s">
+        <v>51</v>
+      </c>
+      <c r="I30" t="s">
+        <v>51</v>
+      </c>
+      <c r="J30" t="s">
+        <v>388</v>
+      </c>
+      <c r="K30" t="s">
+        <v>391</v>
+      </c>
+      <c r="L30" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>396</v>
+      </c>
+      <c r="B31" t="s">
+        <v>398</v>
+      </c>
+      <c r="C31" t="s">
+        <v>392</v>
+      </c>
+      <c r="D31" t="s">
+        <v>394</v>
+      </c>
+      <c r="E31" t="s">
+        <v>393</v>
+      </c>
+      <c r="F31" t="s">
+        <v>395</v>
+      </c>
+      <c r="G31" t="s">
+        <v>400</v>
+      </c>
+      <c r="H31" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" t="s">
+        <v>397</v>
+      </c>
+      <c r="K31" t="s">
+        <v>401</v>
+      </c>
+      <c r="L31" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>405</v>
+      </c>
+      <c r="B32" t="s">
+        <v>407</v>
+      </c>
+      <c r="C32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" t="s">
+        <v>403</v>
+      </c>
+      <c r="E32" t="s">
+        <v>402</v>
+      </c>
+      <c r="F32" t="s">
+        <v>404</v>
+      </c>
+      <c r="G32" t="s">
+        <v>409</v>
+      </c>
+      <c r="H32" t="s">
+        <v>115</v>
+      </c>
+      <c r="I32" t="s">
+        <v>70</v>
+      </c>
+      <c r="J32" t="s">
+        <v>406</v>
+      </c>
+      <c r="K32" t="s">
+        <v>410</v>
+      </c>
+      <c r="L32" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>415</v>
+      </c>
+      <c r="B33" t="s">
+        <v>417</v>
+      </c>
+      <c r="C33" t="s">
+        <v>411</v>
+      </c>
+      <c r="D33" t="s">
+        <v>413</v>
+      </c>
+      <c r="E33" t="s">
+        <v>412</v>
+      </c>
+      <c r="F33" t="s">
+        <v>414</v>
+      </c>
+      <c r="G33" t="s">
+        <v>419</v>
+      </c>
+      <c r="H33" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" t="s">
+        <v>70</v>
+      </c>
+      <c r="J33" t="s">
+        <v>416</v>
+      </c>
+      <c r="K33" t="s">
+        <v>420</v>
+      </c>
+      <c r="L33" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>425</v>
+      </c>
+      <c r="B34" t="s">
+        <v>427</v>
+      </c>
+      <c r="C34" t="s">
+        <v>421</v>
+      </c>
+      <c r="D34" t="s">
+        <v>423</v>
+      </c>
+      <c r="E34" t="s">
+        <v>422</v>
+      </c>
+      <c r="F34" t="s">
+        <v>424</v>
+      </c>
+      <c r="G34" t="s">
+        <v>429</v>
+      </c>
+      <c r="H34" t="s">
+        <v>248</v>
+      </c>
+      <c r="I34" t="s">
+        <v>147</v>
+      </c>
+      <c r="J34" t="s">
+        <v>426</v>
+      </c>
+      <c r="K34" t="s">
+        <v>430</v>
+      </c>
+      <c r="L34" t="s">
+        <v>428</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1428,7 +3028,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A8C0A6-A5D7-4843-BF59-F8CA009F27C6}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -1814,6 +3414,52 @@
       </c>
       <c r="P9" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>444</v>
+      </c>
+      <c r="B10" t="s">
+        <v>446</v>
+      </c>
+      <c r="C10" t="s">
+        <v>440</v>
+      </c>
+      <c r="D10" t="s">
+        <v>442</v>
+      </c>
+      <c r="E10" t="s">
+        <v>441</v>
+      </c>
+      <c r="F10"/>
+      <c r="G10" t="s">
+        <v>443</v>
+      </c>
+      <c r="H10" t="s">
+        <v>448</v>
+      </c>
+      <c r="I10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10" t="s">
+        <v>445</v>
+      </c>
+      <c r="L10" t="s">
+        <v>449</v>
+      </c>
+      <c r="M10" t="s">
+        <v>447</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" t="s">
+        <v>450</v>
+      </c>
+      <c r="P10" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>